<commit_message>
TA278 sheet update includes TA275,TA277
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupTA278.xlsx
+++ b/src/test/resources/data/jdgroupTA278.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\37601\Documents\JDGroupICBranchWorkSpaces\TA270\JD_IC_TestAutomation\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF4F63C-1941-4C6B-A12B-5CACE9B671B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EABE36-DEBF-4A10-8A52-B930420E14C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-11640" windowWidth="20640" windowHeight="11160" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC_ProductsSortBy++" sheetId="39" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="573">
   <si>
     <t>TCID</t>
   </si>
@@ -1744,9 +1744,6 @@
     <t>1#1#2</t>
   </si>
   <si>
-    <t>Cart redirection to Cart details page</t>
-  </si>
-  <si>
     <t>Cart redirection to cart details page</t>
   </si>
   <si>
@@ -1772,16 +1769,32 @@
   </si>
   <si>
     <t>CartTotal</t>
+  </si>
+  <si>
+    <t>Cart redirection to Cart details page TA275</t>
+  </si>
+  <si>
+    <t>Redeem gift cart with invalid coupon code TA277</t>
+  </si>
+  <si>
+    <t>Registered user add items to cart-Logout to login again and confirm cart TA278</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2038,90 +2051,92 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -11137,7 +11152,7 @@
         <v>226</v>
       </c>
       <c r="E37" s="40" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F37" t="s">
         <v>537</v>
@@ -11169,7 +11184,7 @@
         <v>226</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F38" t="s">
         <v>537</v>
@@ -11188,7 +11203,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="24" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H38" xr:uid="{1B5CFA31-9E7B-4741-BC41-5B115AE4E0B6}">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
@@ -11682,7 +11697,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="24" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D15" r:id="rId1" xr:uid="{9D4B1FC9-6A9A-412C-8C1F-B6BAD4758EDE}"/>
     <hyperlink ref="D16" r:id="rId2" xr:uid="{12BCEA30-26A2-432A-8F91-9F716D9A95AE}"/>
@@ -11696,11 +11711,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J55" sqref="J55"/>
+      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -13270,11 +13285,11 @@
       <c r="A53" s="2">
         <v>30</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="48" t="s">
+        <v>570</v>
+      </c>
+      <c r="D53" s="44" t="s">
         <v>561</v>
-      </c>
-      <c r="D53" s="44" t="s">
-        <v>562</v>
       </c>
       <c r="E53" s="45" t="s">
         <v>64</v>
@@ -13286,18 +13301,18 @@
         <v>409</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="2">
         <v>31</v>
       </c>
-      <c r="B54" s="45" t="s">
-        <v>564</v>
+      <c r="B54" s="48" t="s">
+        <v>571</v>
       </c>
       <c r="D54" s="45" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E54" s="46" t="s">
         <v>64</v>
@@ -13309,18 +13324,18 @@
         <v>409</v>
       </c>
       <c r="I54" s="45" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="55" spans="1:13" s="3" customFormat="1">
       <c r="A55" s="3">
         <v>32</v>
       </c>
-      <c r="B55" s="47" t="s">
-        <v>567</v>
+      <c r="B55" s="49" t="s">
+        <v>572</v>
       </c>
       <c r="D55" s="47" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E55" s="47" t="s">
         <v>94</v>
@@ -13338,13 +13353,13 @@
         <v>409</v>
       </c>
       <c r="K55" s="47" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="L55" s="47" t="s">
         <v>384</v>
       </c>
       <c r="M55" s="47" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
   </sheetData>
@@ -15635,8 +15650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D587903-CE57-4C59-A6DB-CB734331903C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -15657,7 +15672,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>